<commit_message>
No actual changes. It was MS.
</commit_message>
<xml_diff>
--- a/app/_Doc/DataModel-Spec.xlsx
+++ b/app/_Doc/DataModel-Spec.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Исходные данные, поступающие из сторонних хранилищ</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>PRIMARY KEY (`AdjDate`)</t>
-  </si>
-  <si>
-    <t>(</t>
   </si>
   <si>
     <t>CREATE TABLE</t>
@@ -81,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -468,7 +465,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -539,7 +536,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +559,7 @@
     <row r="2" spans="1:16" s="6" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -579,13 +576,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
       <c r="P4" t="s">
         <v>10</v>
@@ -602,7 +596,7 @@
         <v>9</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -616,10 +610,10 @@
         <v>9</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -629,7 +623,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve docs and comments
</commit_message>
<xml_diff>
--- a/app/_Doc/DataModel-Spec.xlsx
+++ b/app/_Doc/DataModel-Spec.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="7920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="InboundPrincipal" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="InboundResponse" sheetId="4" r:id="rId3"/>
     <sheet name="Secondary" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
   <si>
     <t>Исходные данные, поступающие из сторонних хранилищ</t>
   </si>
@@ -73,13 +73,181 @@
   </si>
   <si>
     <t>Диапазон копирования</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>-- Структура таблицы `User`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PRIMARY KEY (`ID`)</t>
+  </si>
+  <si>
+    <t>) ENGINE=InnoDB DEFAULT CHARSET=utf8 AUTO_INCREMENT=1 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `ID`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AUTO_INCREMENT,</t>
+  </si>
+  <si>
+    <t>INT(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `Other`</t>
+  </si>
+  <si>
+    <t>TEXT,</t>
+  </si>
+  <si>
+    <t>CREATE TABLE IF NOT EXISTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `User`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `USER`</t>
+  </si>
+  <si>
+    <t>SQL представление</t>
+  </si>
+  <si>
+    <t>Контрагенты по договору НСЖ</t>
+  </si>
+  <si>
+    <t>(добавить реквизиты по контрагенту: тел, почта, ФИО, etc.)</t>
+  </si>
+  <si>
+    <t>-- Структура таблицы `BillingPlan`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TABLE IF NOT EXISTS </t>
+  </si>
+  <si>
+    <t>`BillingPlan`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `AgreementID`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `Active`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tinyint(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEFAULT '1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `PlanDate`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `ToPay`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> decimal(20,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `Currency`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEFAULT 'UAH',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  FOREIGN KEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REFERENCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `Agreement`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (`ID`)</t>
+  </si>
+  <si>
+    <t>Валюта: UAH, EUR, USD</t>
+  </si>
+  <si>
+    <t>Состояние ППО: активен (1); закрыт (0).</t>
+  </si>
+  <si>
+    <t>Пункт Плана Оплат (ППО)</t>
+  </si>
+  <si>
+    <t>-- Структура таблицы `Agreement`</t>
+  </si>
+  <si>
+    <t>`Agreement`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `Insured`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `Insurant`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (`Insured`)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (`ID`),</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (`Insurant`)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PRIMARY KEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PRIMARY KEY </t>
+  </si>
+  <si>
+    <t>(`ID`),</t>
+  </si>
+  <si>
+    <t>(`AgreementID`)</t>
+  </si>
+  <si>
+    <t>Договор действующий (1); приостановлен/расторгнут (0).</t>
+  </si>
+  <si>
+    <t>Договор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `Number`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  `Series`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char(2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +292,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -159,9 +340,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,7 +648,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -493,21 +676,417 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="1.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="1.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="1.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="1.28515625" customWidth="1"/>
+    <col min="12" max="12" width="1.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>42</v>
+      </c>
+      <c r="O25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" t="s">
+        <v>52</v>
+      </c>
+      <c r="K30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="C42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" t="s">
+        <v>51</v>
+      </c>
+      <c r="I47" t="s">
+        <v>29</v>
+      </c>
+      <c r="K47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48" t="s">
+        <v>51</v>
+      </c>
+      <c r="I48" t="s">
+        <v>29</v>
+      </c>
+      <c r="K48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -535,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>